<commit_message>
Add site near Karasjok
</commit_message>
<xml_diff>
--- a/data/tana_subcatchments_2021.xlsx
+++ b/data/tana_subcatchments_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Benoit_D\QUANTOM\quantom\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3961566-6EBF-4890-B723-0A1E3E5FF1E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF5A735-0E07-49E8-94C5-F5C0DFD0214A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{2822E0BF-5117-4FAB-90B3-30C38FEC31F4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Vuomajeaggi</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>Karasjok</t>
+  </si>
+  <si>
+    <t>Approximate location near Karasjok. Taken from https://helikopter.flights/quotes/Price_Taxi_Alta,Norge_Karasjokkommune,Norge.pdf</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774089E4-C2E8-4F20-B878-D16A187B0369}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -676,6 +682,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>69.444800000000001</v>
+      </c>
+      <c r="C14">
+        <v>25.386399999999998</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Use co-ords supplied by Helitrans
</commit_message>
<xml_diff>
--- a/data/tana_subcatchments_2021.xlsx
+++ b/data/tana_subcatchments_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Benoit_D\QUANTOM\quantom\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF5A735-0E07-49E8-94C5-F5C0DFD0214A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7189D0-8D60-4457-8525-D93FC9C653B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{2822E0BF-5117-4FAB-90B3-30C38FEC31F4}"/>
   </bookViews>
@@ -93,10 +93,10 @@
     <t>comment</t>
   </si>
   <si>
-    <t>Karasjok</t>
-  </si>
-  <si>
-    <t>Approximate location near Karasjok. Taken from https://helikopter.flights/quotes/Price_Taxi_Alta,Norge_Karasjokkommune,Norge.pdf</t>
+    <t>Karasjok Camping</t>
+  </si>
+  <si>
+    <t>Suggested by Ann Kristin from Helitrans in e-mail received 02.09.2021</t>
   </si>
 </sst>
 </file>
@@ -471,15 +471,16 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="22.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
@@ -687,10 +688,10 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <v>69.444800000000001</v>
+        <v>69.467986997867399</v>
       </c>
       <c r="C14">
-        <v>25.386399999999998</v>
+        <v>25.487036705017001</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>

</xml_diff>